<commit_message>
new xlsx file and corresponding code changes.
</commit_message>
<xml_diff>
--- a/src/Graphs/correlation_matrix.xlsx
+++ b/src/Graphs/correlation_matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ad18d7acc2411bc9/Documents/Python-Projects/Credit-Project/src/Graphs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_5339E03C5648F00F62355476585DCE3A8747A5F9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0570DCC8-FFCC-42F9-9B66-DD897AC65FE5}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_278990ACD370D7342B583811595ED87656CD2BBE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BFEC40EE-F187-4D71-AACD-56B9EABEA0D1}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -95,10 +95,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,13 +107,6 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -151,62 +141,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -517,8 +464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -598,73 +545,73 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
         <v>-0.21916069822921161</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2">
         <v>-0.1081394102780129</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2">
         <v>0.14471279755733671</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2">
         <v>-0.27121433213471791</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2">
         <v>-0.29638210099648238</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2">
         <v>-0.28612295390311437</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2">
         <v>-0.26746000963939298</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J2">
         <v>-0.24941139482410929</v>
       </c>
-      <c r="K2" s="2">
+      <c r="K2">
         <v>-0.23519539948542489</v>
       </c>
-      <c r="L2" s="2">
+      <c r="L2">
         <v>0.28542986496499001</v>
       </c>
-      <c r="M2" s="2">
+      <c r="M2">
         <v>0.27831436399776099</v>
       </c>
-      <c r="N2" s="2">
+      <c r="N2">
         <v>0.28323578358168422</v>
       </c>
-      <c r="O2" s="2">
+      <c r="O2">
         <v>0.29398762371598491</v>
       </c>
-      <c r="P2" s="2">
+      <c r="P2">
         <v>0.29556233765823159</v>
       </c>
-      <c r="Q2" s="2">
+      <c r="Q2">
         <v>0.29038895064794751</v>
       </c>
-      <c r="R2" s="2">
+      <c r="R2">
         <v>0.1952359152322094</v>
       </c>
-      <c r="S2" s="2">
+      <c r="S2">
         <v>0.1784079536837051</v>
       </c>
-      <c r="T2" s="2">
+      <c r="T2">
         <v>0.210166747723388</v>
       </c>
-      <c r="U2" s="2">
+      <c r="U2">
         <v>0.20324241022458289</v>
       </c>
-      <c r="V2" s="2">
+      <c r="V2">
         <v>0.21720243239549611</v>
       </c>
-      <c r="W2" s="2">
+      <c r="W2">
         <v>0.2195953686044175</v>
       </c>
-      <c r="X2" s="2">
+      <c r="X2">
         <v>-0.1535198763935072</v>
       </c>
     </row>
@@ -672,73 +619,73 @@
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3">
         <v>-0.21916069822921161</v>
       </c>
-      <c r="C3" s="2">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2">
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
         <v>-0.14346434041144779</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3">
         <v>0.17506066148808549</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3">
         <v>0.1053639979353248</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3">
         <v>0.1215655524706702</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3">
         <v>0.1140249028571366</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3">
         <v>0.1087934561527877</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3">
         <v>9.7520160630195626E-2</v>
       </c>
-      <c r="K3" s="2">
+      <c r="K3">
         <v>8.2315986377468217E-2</v>
       </c>
-      <c r="L3" s="2">
+      <c r="L3">
         <v>2.3581180737114391E-2</v>
       </c>
-      <c r="M3" s="2">
+      <c r="M3">
         <v>1.8748770808322431E-2</v>
       </c>
-      <c r="N3" s="2">
+      <c r="N3">
         <v>1.3002400711998921E-2</v>
       </c>
-      <c r="O3" s="2">
+      <c r="O3">
         <v>-4.5134530874911061E-4</v>
       </c>
-      <c r="P3" s="2">
+      <c r="P3">
         <v>-7.5665030468417107E-3</v>
       </c>
-      <c r="Q3" s="2">
+      <c r="Q3">
         <v>-9.0989546974553723E-3</v>
       </c>
-      <c r="R3" s="2">
+      <c r="R3">
         <v>-3.7456183913116482E-2</v>
       </c>
-      <c r="S3" s="2">
+      <c r="S3">
         <v>-3.0038186562838982E-2</v>
       </c>
-      <c r="T3" s="2">
+      <c r="T3">
         <v>-3.9943140867107353E-2</v>
       </c>
-      <c r="U3" s="2">
+      <c r="U3">
         <v>-3.8218166111341469E-2</v>
       </c>
-      <c r="V3" s="2">
+      <c r="V3">
         <v>-4.0358454928196917E-2</v>
       </c>
-      <c r="W3" s="2">
+      <c r="W3">
         <v>-3.7199903089169373E-2</v>
       </c>
-      <c r="X3" s="2">
+      <c r="X3">
         <v>2.8006077656250201E-2</v>
       </c>
     </row>
@@ -746,73 +693,73 @@
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4">
         <v>-0.1081394102780129</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4">
         <v>-0.14346434041144779</v>
       </c>
-      <c r="D4" s="2">
-        <v>1</v>
-      </c>
-      <c r="E4" s="2">
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
         <v>-0.41416991848813439</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4">
         <v>1.991719048342673E-2</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4">
         <v>2.4199067281193389E-2</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4">
         <v>3.268767333723676E-2</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4">
         <v>3.3121548914055277E-2</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4">
         <v>3.5629170366555538E-2</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4">
         <v>3.4344765997445452E-2</v>
       </c>
-      <c r="L4" s="2">
+      <c r="L4">
         <v>-2.347180191012958E-2</v>
       </c>
-      <c r="M4" s="2">
+      <c r="M4">
         <v>-2.160177985903031E-2</v>
       </c>
-      <c r="N4" s="2">
+      <c r="N4">
         <v>-2.490945102250099E-2</v>
       </c>
-      <c r="O4" s="2">
+      <c r="O4">
         <v>-2.334384691537595E-2</v>
       </c>
-      <c r="P4" s="2">
+      <c r="P4">
         <v>-2.5393397991274679E-2</v>
       </c>
-      <c r="Q4" s="2">
+      <c r="Q4">
         <v>-2.1206824800079151E-2</v>
       </c>
-      <c r="R4" s="2">
+      <c r="R4">
         <v>-5.9789997808353231E-3</v>
       </c>
-      <c r="S4" s="2">
+      <c r="S4">
         <v>-8.0927028377798891E-3</v>
       </c>
-      <c r="T4" s="2">
+      <c r="T4">
         <v>-3.541351946757382E-3</v>
       </c>
-      <c r="U4" s="2">
+      <c r="U4">
         <v>-1.265927889271911E-2</v>
       </c>
-      <c r="V4" s="2">
+      <c r="V4">
         <v>-1.2047569155652471E-3</v>
       </c>
-      <c r="W4" s="2">
+      <c r="W4">
         <v>-6.640941925653474E-3</v>
       </c>
-      <c r="X4" s="2">
+      <c r="X4">
         <v>-2.4339215683404442E-2</v>
       </c>
     </row>
@@ -820,73 +767,73 @@
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5">
         <v>0.14471279755733671</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5">
         <v>0.17506066148808549</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5">
         <v>-0.41416991848813439</v>
       </c>
-      <c r="E5" s="2">
-        <v>1</v>
-      </c>
-      <c r="F5" s="2">
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
         <v>-3.9447376184119809E-2</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5">
         <v>-5.0147776206855219E-2</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5">
         <v>-5.3048437258163342E-2</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5">
         <v>-4.9721673995377233E-2</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5">
         <v>-5.3825976413085778E-2</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K5">
         <v>-4.8773426428324211E-2</v>
       </c>
-      <c r="L5" s="2">
+      <c r="L5">
         <v>5.6238533260566589E-2</v>
       </c>
-      <c r="M5" s="2">
+      <c r="M5">
         <v>5.4283074350342443E-2</v>
       </c>
-      <c r="N5" s="2">
+      <c r="N5">
         <v>5.3709705178660243E-2</v>
       </c>
-      <c r="O5" s="2">
+      <c r="O5">
         <v>5.1353093243321428E-2</v>
       </c>
-      <c r="P5" s="2">
+      <c r="P5">
         <v>4.9345048112611777E-2</v>
       </c>
-      <c r="Q5" s="2">
+      <c r="Q5">
         <v>4.7612677990511262E-2</v>
       </c>
-      <c r="R5" s="2">
+      <c r="R5">
         <v>2.614667905698919E-2</v>
       </c>
-      <c r="S5" s="2">
+      <c r="S5">
         <v>2.1784893392614191E-2</v>
       </c>
-      <c r="T5" s="2">
+      <c r="T5">
         <v>2.9247353045011429E-2</v>
       </c>
-      <c r="U5" s="2">
+      <c r="U5">
         <v>2.137900561558986E-2</v>
       </c>
-      <c r="V5" s="2">
+      <c r="V5">
         <v>2.2849973558558761E-2</v>
       </c>
-      <c r="W5" s="2">
+      <c r="W5">
         <v>1.9478152969869801E-2</v>
       </c>
-      <c r="X5" s="2">
+      <c r="X5">
         <v>1.3889834301962891E-2</v>
       </c>
     </row>
@@ -894,73 +841,73 @@
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6">
         <v>-0.27121433213471791</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6">
         <v>0.1053639979353248</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6">
         <v>1.991719048342673E-2</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6">
         <v>-3.9447376184119809E-2</v>
       </c>
-      <c r="F6" s="2">
-        <v>1</v>
-      </c>
-      <c r="G6" s="2">
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
         <v>0.67216438254831423</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6">
         <v>0.57424509262043788</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6">
         <v>0.53884062687123335</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6">
         <v>0.50942606366544463</v>
       </c>
-      <c r="K6" s="2">
+      <c r="K6">
         <v>0.4745530860641517</v>
       </c>
-      <c r="L6" s="2">
+      <c r="L6">
         <v>0.18706843147380109</v>
       </c>
-      <c r="M6" s="2">
+      <c r="M6">
         <v>0.18985910889354429</v>
       </c>
-      <c r="N6" s="2">
+      <c r="N6">
         <v>0.17978528216681919</v>
       </c>
-      <c r="O6" s="2">
+      <c r="O6">
         <v>0.1791247706258787</v>
       </c>
-      <c r="P6" s="2">
+      <c r="P6">
         <v>0.18063462540120859</v>
       </c>
-      <c r="Q6" s="2">
+      <c r="Q6">
         <v>0.17698029564143791</v>
       </c>
-      <c r="R6" s="2">
+      <c r="R6">
         <v>-7.9268711185419505E-2</v>
       </c>
-      <c r="S6" s="2">
+      <c r="S6">
         <v>-7.0100521193938697E-2</v>
       </c>
-      <c r="T6" s="2">
+      <c r="T6">
         <v>-7.0560837670354787E-2</v>
       </c>
-      <c r="U6" s="2">
+      <c r="U6">
         <v>-6.400488888773119E-2</v>
       </c>
-      <c r="V6" s="2">
+      <c r="V6">
         <v>-5.8189885949777302E-2</v>
       </c>
-      <c r="W6" s="2">
+      <c r="W6">
         <v>-5.8673214376070433E-2</v>
       </c>
-      <c r="X6" s="2">
+      <c r="X6">
         <v>0.32479372847862242</v>
       </c>
     </row>
@@ -968,73 +915,73 @@
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7">
         <v>-0.29638210099648238</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7">
         <v>0.1215655524706702</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7">
         <v>2.4199067281193389E-2</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7">
         <v>-5.0147776206855219E-2</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7">
         <v>0.67216438254831423</v>
       </c>
-      <c r="G7" s="2">
-        <v>1</v>
-      </c>
-      <c r="H7" s="2">
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
         <v>0.7665516829341017</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7">
         <v>0.66206713102395909</v>
       </c>
-      <c r="J7" s="2">
+      <c r="J7">
         <v>0.62278024537687027</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K7">
         <v>0.57550086177930537</v>
       </c>
-      <c r="L7" s="2">
+      <c r="L7">
         <v>0.23488652660358381</v>
       </c>
-      <c r="M7" s="2">
+      <c r="M7">
         <v>0.23525694274352649</v>
       </c>
-      <c r="N7" s="2">
+      <c r="N7">
         <v>0.22414585503162601</v>
       </c>
-      <c r="O7" s="2">
+      <c r="O7">
         <v>0.22223651161283831</v>
       </c>
-      <c r="P7" s="2">
+      <c r="P7">
         <v>0.2213483730334278</v>
       </c>
-      <c r="Q7" s="2">
+      <c r="Q7">
         <v>0.21940335128667951</v>
       </c>
-      <c r="R7" s="2">
+      <c r="R7">
         <v>-8.0700709810166957E-2</v>
       </c>
-      <c r="S7" s="2">
+      <c r="S7">
         <v>-5.8989999034612828E-2</v>
       </c>
-      <c r="T7" s="2">
+      <c r="T7">
         <v>-5.5901231300968322E-2</v>
       </c>
-      <c r="U7" s="2">
+      <c r="U7">
         <v>-4.6858411513545577E-2</v>
       </c>
-      <c r="V7" s="2">
+      <c r="V7">
         <v>-3.7093079770128587E-2</v>
       </c>
-      <c r="W7" s="2">
+      <c r="W7">
         <v>-3.650037552721859E-2</v>
       </c>
-      <c r="X7" s="2">
+      <c r="X7">
         <v>0.26355120167216778</v>
       </c>
     </row>
@@ -1042,73 +989,73 @@
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8">
         <v>-0.28612295390311437</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8">
         <v>0.1140249028571366</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8">
         <v>3.268767333723676E-2</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8">
         <v>-5.3048437258163342E-2</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8">
         <v>0.57424509262043788</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8">
         <v>0.7665516829341017</v>
       </c>
-      <c r="H8" s="2">
-        <v>1</v>
-      </c>
-      <c r="I8" s="2">
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
         <v>0.77735887330127262</v>
       </c>
-      <c r="J8" s="2">
+      <c r="J8">
         <v>0.68677451099478526</v>
       </c>
-      <c r="K8" s="2">
+      <c r="K8">
         <v>0.63268359271844554</v>
       </c>
-      <c r="L8" s="2">
+      <c r="L8">
         <v>0.20847288868976011</v>
       </c>
-      <c r="M8" s="2">
+      <c r="M8">
         <v>0.2372945344029275</v>
       </c>
-      <c r="N8" s="2">
+      <c r="N8">
         <v>0.22749432669556149</v>
       </c>
-      <c r="O8" s="2">
+      <c r="O8">
         <v>0.22720228070078949</v>
       </c>
-      <c r="P8" s="2">
+      <c r="P8">
         <v>0.22514519307202241</v>
       </c>
-      <c r="Q8" s="2">
+      <c r="Q8">
         <v>0.2223267374363066</v>
       </c>
-      <c r="R8" s="2">
+      <c r="R8">
         <v>1.2948143319480221E-3</v>
       </c>
-      <c r="S8" s="2">
+      <c r="S8">
         <v>-6.6793395665513289E-2</v>
       </c>
-      <c r="T8" s="2">
+      <c r="T8">
         <v>-5.3310779586101961E-2</v>
       </c>
-      <c r="U8" s="2">
+      <c r="U8">
         <v>-4.606653388796151E-2</v>
       </c>
-      <c r="V8" s="2">
+      <c r="V8">
         <v>-3.5863070561361177E-2</v>
       </c>
-      <c r="W8" s="2">
+      <c r="W8">
         <v>-3.5861083718773168E-2</v>
       </c>
-      <c r="X8" s="2">
+      <c r="X8">
         <v>0.2352525137249171</v>
       </c>
     </row>
@@ -1116,73 +1063,73 @@
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9">
         <v>-0.26746000963939298</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9">
         <v>0.1087934561527877</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9">
         <v>3.3121548914055277E-2</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9">
         <v>-4.9721673995377233E-2</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9">
         <v>0.53884062687123335</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9">
         <v>0.66206713102395909</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9">
         <v>0.77735887330127262</v>
       </c>
-      <c r="I9" s="2">
-        <v>1</v>
-      </c>
-      <c r="J9" s="2">
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
         <v>0.81983531148681577</v>
       </c>
-      <c r="K9" s="2">
+      <c r="K9">
         <v>0.71644948158078448</v>
       </c>
-      <c r="L9" s="2">
+      <c r="L9">
         <v>0.2028120693874492</v>
       </c>
-      <c r="M9" s="2">
+      <c r="M9">
         <v>0.22581631606808819</v>
       </c>
-      <c r="N9" s="2">
+      <c r="N9">
         <v>0.24498313796206861</v>
       </c>
-      <c r="O9" s="2">
+      <c r="O9">
         <v>0.24591720419843821</v>
       </c>
-      <c r="P9" s="2">
+      <c r="P9">
         <v>0.24290205842488449</v>
       </c>
-      <c r="Q9" s="2">
+      <c r="Q9">
         <v>0.23915412960583929</v>
       </c>
-      <c r="R9" s="2">
+      <c r="R9">
         <v>-9.3621357544022323E-3</v>
       </c>
-      <c r="S9" s="2">
+      <c r="S9">
         <v>-1.9436566079039941E-3</v>
       </c>
-      <c r="T9" s="2">
+      <c r="T9">
         <v>-6.9235203567686907E-2</v>
       </c>
-      <c r="U9" s="2">
+      <c r="U9">
         <v>-4.3461429655394422E-2</v>
       </c>
-      <c r="V9" s="2">
+      <c r="V9">
         <v>-3.3589534748121493E-2</v>
       </c>
-      <c r="W9" s="2">
+      <c r="W9">
         <v>-2.656508796765087E-2</v>
       </c>
-      <c r="X9" s="2">
+      <c r="X9">
         <v>0.21661363684242391</v>
       </c>
     </row>
@@ -1190,73 +1137,73 @@
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10">
         <v>-0.24941139482410929</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10">
         <v>9.7520160630195626E-2</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10">
         <v>3.5629170366555538E-2</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10">
         <v>-5.3825976413085778E-2</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10">
         <v>0.50942606366544463</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10">
         <v>0.62278024537687027</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10">
         <v>0.68677451099478526</v>
       </c>
-      <c r="I10" s="2">
+      <c r="I10">
         <v>0.81983531148681577</v>
       </c>
-      <c r="J10" s="2">
-        <v>1</v>
-      </c>
-      <c r="K10" s="2">
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
         <v>0.81690016041767533</v>
       </c>
-      <c r="L10" s="2">
+      <c r="L10">
         <v>0.20668396424409591</v>
       </c>
-      <c r="M10" s="2">
+      <c r="M10">
         <v>0.2269132669915285</v>
       </c>
-      <c r="N10" s="2">
+      <c r="N10">
         <v>0.24333468092023641</v>
       </c>
-      <c r="O10" s="2">
+      <c r="O10">
         <v>0.271915006998107</v>
       </c>
-      <c r="P10" s="2">
+      <c r="P10">
         <v>0.26978309015113511</v>
       </c>
-      <c r="Q10" s="2">
+      <c r="Q10">
         <v>0.26250925166841732</v>
       </c>
-      <c r="R10" s="2">
+      <c r="R10">
         <v>-6.0887571388422313E-3</v>
       </c>
-      <c r="S10" s="2">
+      <c r="S10">
         <v>-3.1913323070528149E-3</v>
       </c>
-      <c r="T10" s="2">
+      <c r="T10">
         <v>9.0623626815555386E-3</v>
       </c>
-      <c r="U10" s="2">
+      <c r="U10">
         <v>-5.829886530946838E-2</v>
       </c>
-      <c r="V10" s="2">
+      <c r="V10">
         <v>-3.333650421280087E-2</v>
       </c>
-      <c r="W10" s="2">
+      <c r="W10">
         <v>-2.302745098759577E-2</v>
       </c>
-      <c r="X10" s="2">
+      <c r="X10">
         <v>0.20414891387616449</v>
       </c>
     </row>
@@ -1264,73 +1211,73 @@
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11">
         <v>-0.23519539948542489</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11">
         <v>8.2315986377468217E-2</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11">
         <v>3.4344765997445452E-2</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11">
         <v>-4.8773426428324211E-2</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11">
         <v>0.4745530860641517</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11">
         <v>0.57550086177930537</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11">
         <v>0.63268359271844554</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I11">
         <v>0.71644948158078448</v>
       </c>
-      <c r="J11" s="2">
+      <c r="J11">
         <v>0.81690016041767533</v>
       </c>
-      <c r="K11" s="2">
-        <v>1</v>
-      </c>
-      <c r="L11" s="2">
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
         <v>0.20737313129566121</v>
       </c>
-      <c r="M11" s="2">
+      <c r="M11">
         <v>0.22692443093066761</v>
       </c>
-      <c r="N11" s="2">
+      <c r="N11">
         <v>0.2411811460423216</v>
       </c>
-      <c r="O11" s="2">
+      <c r="O11">
         <v>0.26635606903390779</v>
       </c>
-      <c r="P11" s="2">
+      <c r="P11">
         <v>0.29089374494860698</v>
       </c>
-      <c r="Q11" s="2">
+      <c r="Q11">
         <v>0.28509099069256871</v>
       </c>
-      <c r="R11" s="2">
+      <c r="R11">
         <v>-1.496289043318072E-3</v>
       </c>
-      <c r="S11" s="2">
+      <c r="S11">
         <v>-5.2232681440545856E-3</v>
       </c>
-      <c r="T11" s="2">
+      <c r="T11">
         <v>5.8337741928969761E-3</v>
       </c>
-      <c r="U11" s="2">
+      <c r="U11">
         <v>1.9017863282441622E-2</v>
       </c>
-      <c r="V11" s="2">
+      <c r="V11">
         <v>-4.6433641072996593E-2</v>
       </c>
-      <c r="W11" s="2">
+      <c r="W11">
         <v>-2.529933846228534E-2</v>
       </c>
-      <c r="X11" s="2">
+      <c r="X11">
         <v>0.18686636165354609</v>
       </c>
     </row>
@@ -1338,73 +1285,73 @@
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12">
         <v>0.28542986496499001</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12">
         <v>2.3581180737114391E-2</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12">
         <v>-2.347180191012958E-2</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12">
         <v>5.6238533260566589E-2</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12">
         <v>0.18706843147380109</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12">
         <v>0.23488652660358381</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12">
         <v>0.20847288868976011</v>
       </c>
-      <c r="I12" s="2">
+      <c r="I12">
         <v>0.2028120693874492</v>
       </c>
-      <c r="J12" s="2">
+      <c r="J12">
         <v>0.20668396424409591</v>
       </c>
-      <c r="K12" s="2">
+      <c r="K12">
         <v>0.20737313129566121</v>
       </c>
-      <c r="L12" s="2">
-        <v>1</v>
-      </c>
-      <c r="M12" s="2">
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
         <v>0.95148367275181356</v>
       </c>
-      <c r="N12" s="2">
+      <c r="N12">
         <v>0.89227852912717609</v>
       </c>
-      <c r="O12" s="2">
+      <c r="O12">
         <v>0.86027218902930946</v>
       </c>
-      <c r="P12" s="2">
+      <c r="P12">
         <v>0.82977860583300134</v>
       </c>
-      <c r="Q12" s="2">
+      <c r="Q12">
         <v>0.80265018855284553</v>
       </c>
-      <c r="R12" s="2">
+      <c r="R12">
         <v>0.14027727757532421</v>
       </c>
-      <c r="S12" s="2">
+      <c r="S12">
         <v>9.9355034972768305E-2</v>
       </c>
-      <c r="T12" s="2">
+      <c r="T12">
         <v>0.15688713847568511</v>
       </c>
-      <c r="U12" s="2">
+      <c r="U12">
         <v>0.15830253328353999</v>
       </c>
-      <c r="V12" s="2">
+      <c r="V12">
         <v>0.16702571208291589</v>
       </c>
-      <c r="W12" s="2">
+      <c r="W12">
         <v>0.17934112200688429</v>
       </c>
-      <c r="X12" s="2">
+      <c r="X12">
         <v>-1.9644197143221558E-2</v>
       </c>
     </row>
@@ -1412,73 +1359,73 @@
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13">
         <v>0.27831436399776099</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13">
         <v>1.8748770808322431E-2</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13">
         <v>-2.160177985903031E-2</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13">
         <v>5.4283074350342443E-2</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13">
         <v>0.18985910889354429</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13">
         <v>0.23525694274352649</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H13">
         <v>0.2372945344029275</v>
       </c>
-      <c r="I13" s="2">
+      <c r="I13">
         <v>0.22581631606808819</v>
       </c>
-      <c r="J13" s="2">
+      <c r="J13">
         <v>0.2269132669915285</v>
       </c>
-      <c r="K13" s="2">
+      <c r="K13">
         <v>0.22692443093066761</v>
       </c>
-      <c r="L13" s="2">
+      <c r="L13">
         <v>0.95148367275181356</v>
       </c>
-      <c r="M13" s="2">
-        <v>1</v>
-      </c>
-      <c r="N13" s="2">
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13">
         <v>0.92832625927148549</v>
       </c>
-      <c r="O13" s="2">
+      <c r="O13">
         <v>0.89248229125772094</v>
       </c>
-      <c r="P13" s="2">
+      <c r="P13">
         <v>0.859778307271445</v>
       </c>
-      <c r="Q13" s="2">
+      <c r="Q13">
         <v>0.83159355910182131</v>
       </c>
-      <c r="R13" s="2">
+      <c r="R13">
         <v>0.28036535701409993</v>
       </c>
-      <c r="S13" s="2">
+      <c r="S13">
         <v>0.10085087751752871</v>
       </c>
-      <c r="T13" s="2">
+      <c r="T13">
         <v>0.15071819370167511</v>
       </c>
-      <c r="U13" s="2">
+      <c r="U13">
         <v>0.14739810422001151</v>
       </c>
-      <c r="V13" s="2">
+      <c r="V13">
         <v>0.15795741162396421</v>
       </c>
-      <c r="W13" s="2">
+      <c r="W13">
         <v>0.17425616563434329</v>
       </c>
-      <c r="X13" s="2">
+      <c r="X13">
         <v>-1.419321808821576E-2</v>
       </c>
     </row>
@@ -1486,73 +1433,73 @@
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14">
         <v>0.28323578358168422</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14">
         <v>1.3002400711998921E-2</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14">
         <v>-2.490945102250099E-2</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14">
         <v>5.3709705178660243E-2</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14">
         <v>0.17978528216681919</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G14">
         <v>0.22414585503162601</v>
       </c>
-      <c r="H14" s="2">
+      <c r="H14">
         <v>0.22749432669556149</v>
       </c>
-      <c r="I14" s="2">
+      <c r="I14">
         <v>0.24498313796206861</v>
       </c>
-      <c r="J14" s="2">
+      <c r="J14">
         <v>0.24333468092023641</v>
       </c>
-      <c r="K14" s="2">
+      <c r="K14">
         <v>0.2411811460423216</v>
       </c>
-      <c r="L14" s="2">
+      <c r="L14">
         <v>0.89227852912717609</v>
       </c>
-      <c r="M14" s="2">
+      <c r="M14">
         <v>0.92832625927148549</v>
       </c>
-      <c r="N14" s="2">
-        <v>1</v>
-      </c>
-      <c r="O14" s="2">
+      <c r="N14">
+        <v>1</v>
+      </c>
+      <c r="O14">
         <v>0.92396945659098229</v>
       </c>
-      <c r="P14" s="2">
+      <c r="P14">
         <v>0.88390969736201552</v>
       </c>
-      <c r="Q14" s="2">
+      <c r="Q14">
         <v>0.85332009059404679</v>
       </c>
-      <c r="R14" s="2">
+      <c r="R14">
         <v>0.24433523760815989</v>
       </c>
-      <c r="S14" s="2">
+      <c r="S14">
         <v>0.31693597717969058</v>
       </c>
-      <c r="T14" s="2">
+      <c r="T14">
         <v>0.1300111816244208</v>
       </c>
-      <c r="U14" s="2">
+      <c r="U14">
         <v>0.14340460499244431</v>
       </c>
-      <c r="V14" s="2">
+      <c r="V14">
         <v>0.17971235040649311</v>
       </c>
-      <c r="W14" s="2">
+      <c r="W14">
         <v>0.1823259661520534</v>
       </c>
-      <c r="X14" s="2">
+      <c r="X14">
         <v>-1.4075518043214731E-2</v>
       </c>
     </row>
@@ -1560,73 +1507,73 @@
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15">
         <v>0.29398762371598491</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15">
         <v>-4.5134530874911061E-4</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15">
         <v>-2.334384691537595E-2</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15">
         <v>5.1353093243321428E-2</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15">
         <v>0.1791247706258787</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15">
         <v>0.22223651161283831</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H15">
         <v>0.22720228070078949</v>
       </c>
-      <c r="I15" s="2">
+      <c r="I15">
         <v>0.24591720419843821</v>
       </c>
-      <c r="J15" s="2">
+      <c r="J15">
         <v>0.271915006998107</v>
       </c>
-      <c r="K15" s="2">
+      <c r="K15">
         <v>0.26635606903390779</v>
       </c>
-      <c r="L15" s="2">
+      <c r="L15">
         <v>0.86027218902930946</v>
       </c>
-      <c r="M15" s="2">
+      <c r="M15">
         <v>0.89248229125772094</v>
       </c>
-      <c r="N15" s="2">
+      <c r="N15">
         <v>0.92396945659098229</v>
       </c>
-      <c r="O15" s="2">
-        <v>1</v>
-      </c>
-      <c r="P15" s="2">
+      <c r="O15">
+        <v>1</v>
+      </c>
+      <c r="P15">
         <v>0.94013440408800042</v>
       </c>
-      <c r="Q15" s="2">
+      <c r="Q15">
         <v>0.90094095479784209</v>
       </c>
-      <c r="R15" s="2">
+      <c r="R15">
         <v>0.23301185215343709</v>
       </c>
-      <c r="S15" s="2">
+      <c r="S15">
         <v>0.20756372904207551</v>
       </c>
-      <c r="T15" s="2">
+      <c r="T15">
         <v>0.3000225291116479</v>
       </c>
-      <c r="U15" s="2">
+      <c r="U15">
         <v>0.13019140778780799</v>
       </c>
-      <c r="V15" s="2">
+      <c r="V15">
         <v>0.1604330376290044</v>
       </c>
-      <c r="W15" s="2">
+      <c r="W15">
         <v>0.17763699418674461</v>
       </c>
-      <c r="X15" s="2">
+      <c r="X15">
         <v>-1.0156495880289671E-2</v>
       </c>
     </row>
@@ -1634,73 +1581,73 @@
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16">
         <v>0.29556233765823159</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16">
         <v>-7.5665030468417107E-3</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16">
         <v>-2.5393397991274679E-2</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16">
         <v>4.9345048112611777E-2</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16">
         <v>0.18063462540120859</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G16">
         <v>0.2213483730334278</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H16">
         <v>0.22514519307202241</v>
       </c>
-      <c r="I16" s="2">
+      <c r="I16">
         <v>0.24290205842488449</v>
       </c>
-      <c r="J16" s="2">
+      <c r="J16">
         <v>0.26978309015113511</v>
       </c>
-      <c r="K16" s="2">
+      <c r="K16">
         <v>0.29089374494860698</v>
       </c>
-      <c r="L16" s="2">
+      <c r="L16">
         <v>0.82977860583300134</v>
       </c>
-      <c r="M16" s="2">
+      <c r="M16">
         <v>0.859778307271445</v>
       </c>
-      <c r="N16" s="2">
+      <c r="N16">
         <v>0.88390969736201552</v>
       </c>
-      <c r="O16" s="2">
+      <c r="O16">
         <v>0.94013440408800042</v>
       </c>
-      <c r="P16" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q16" s="2">
+      <c r="P16">
+        <v>1</v>
+      </c>
+      <c r="Q16">
         <v>0.94619680705219567</v>
       </c>
-      <c r="R16" s="2">
+      <c r="R16">
         <v>0.21703082377805019</v>
       </c>
-      <c r="S16" s="2">
+      <c r="S16">
         <v>0.18124649105227689</v>
       </c>
-      <c r="T16" s="2">
+      <c r="T16">
         <v>0.25230486173062922</v>
       </c>
-      <c r="U16" s="2">
+      <c r="U16">
         <v>0.29311846318443119</v>
       </c>
-      <c r="V16" s="2">
+      <c r="V16">
         <v>0.14157417995960681</v>
       </c>
-      <c r="W16" s="2">
+      <c r="W16">
         <v>0.1641844503536177</v>
       </c>
-      <c r="X16" s="2">
+      <c r="X16">
         <v>-6.7604638410147791E-3</v>
       </c>
     </row>
@@ -1708,73 +1655,73 @@
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17">
         <v>0.29038895064794751</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17">
         <v>-9.0989546974553723E-3</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17">
         <v>-2.1206824800079151E-2</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17">
         <v>4.7612677990511262E-2</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17">
         <v>0.17698029564143791</v>
       </c>
-      <c r="G17" s="2">
+      <c r="G17">
         <v>0.21940335128667951</v>
       </c>
-      <c r="H17" s="2">
+      <c r="H17">
         <v>0.2223267374363066</v>
       </c>
-      <c r="I17" s="2">
+      <c r="I17">
         <v>0.23915412960583929</v>
       </c>
-      <c r="J17" s="2">
+      <c r="J17">
         <v>0.26250925166841732</v>
       </c>
-      <c r="K17" s="2">
+      <c r="K17">
         <v>0.28509099069256871</v>
       </c>
-      <c r="L17" s="2">
+      <c r="L17">
         <v>0.80265018855284553</v>
       </c>
-      <c r="M17" s="2">
+      <c r="M17">
         <v>0.83159355910182131</v>
       </c>
-      <c r="N17" s="2">
+      <c r="N17">
         <v>0.85332009059404679</v>
       </c>
-      <c r="O17" s="2">
+      <c r="O17">
         <v>0.90094095479784209</v>
       </c>
-      <c r="P17" s="2">
+      <c r="P17">
         <v>0.94619680705219567</v>
       </c>
-      <c r="Q17" s="2">
-        <v>1</v>
-      </c>
-      <c r="R17" s="2">
+      <c r="Q17">
+        <v>1</v>
+      </c>
+      <c r="R17">
         <v>0.199965006163385</v>
       </c>
-      <c r="S17" s="2">
+      <c r="S17">
         <v>0.1726629374180296</v>
       </c>
-      <c r="T17" s="2">
+      <c r="T17">
         <v>0.23376979332693371</v>
       </c>
-      <c r="U17" s="2">
+      <c r="U17">
         <v>0.25023682493343619</v>
       </c>
-      <c r="V17" s="2">
+      <c r="V17">
         <v>0.30772888950115462</v>
       </c>
-      <c r="W17" s="2">
+      <c r="W17">
         <v>0.1154941668516445</v>
       </c>
-      <c r="X17" s="2">
+      <c r="X17">
         <v>-5.3723149148155579E-3</v>
       </c>
     </row>
@@ -1782,73 +1729,73 @@
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18">
         <v>0.1952359152322094</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18">
         <v>-3.7456183913116482E-2</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18">
         <v>-5.9789997808353231E-3</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18">
         <v>2.614667905698919E-2</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18">
         <v>-7.9268711185419505E-2</v>
       </c>
-      <c r="G18" s="2">
+      <c r="G18">
         <v>-8.0700709810166957E-2</v>
       </c>
-      <c r="H18" s="2">
+      <c r="H18">
         <v>1.2948143319480221E-3</v>
       </c>
-      <c r="I18" s="2">
+      <c r="I18">
         <v>-9.3621357544022323E-3</v>
       </c>
-      <c r="J18" s="2">
+      <c r="J18">
         <v>-6.0887571388422313E-3</v>
       </c>
-      <c r="K18" s="2">
+      <c r="K18">
         <v>-1.496289043318072E-3</v>
       </c>
-      <c r="L18" s="2">
+      <c r="L18">
         <v>0.14027727757532421</v>
       </c>
-      <c r="M18" s="2">
+      <c r="M18">
         <v>0.28036535701409993</v>
       </c>
-      <c r="N18" s="2">
+      <c r="N18">
         <v>0.24433523760815989</v>
       </c>
-      <c r="O18" s="2">
+      <c r="O18">
         <v>0.23301185215343709</v>
       </c>
-      <c r="P18" s="2">
+      <c r="P18">
         <v>0.21703082377805019</v>
       </c>
-      <c r="Q18" s="2">
+      <c r="Q18">
         <v>0.199965006163385</v>
       </c>
-      <c r="R18" s="2">
-        <v>1</v>
-      </c>
-      <c r="S18" s="2">
+      <c r="R18">
+        <v>1</v>
+      </c>
+      <c r="S18">
         <v>0.28557552868684261</v>
       </c>
-      <c r="T18" s="2">
+      <c r="T18">
         <v>0.25219113895240292</v>
       </c>
-      <c r="U18" s="2">
+      <c r="U18">
         <v>0.1995579311706798</v>
       </c>
-      <c r="V18" s="2">
+      <c r="V18">
         <v>0.1484592750153427</v>
       </c>
-      <c r="W18" s="2">
+      <c r="W18">
         <v>0.18573525544572639</v>
       </c>
-      <c r="X18" s="2">
+      <c r="X18">
         <v>-7.2929487777851632E-2</v>
       </c>
     </row>
@@ -1856,73 +1803,73 @@
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19">
         <v>0.1784079536837051</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19">
         <v>-3.0038186562838982E-2</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19">
         <v>-8.0927028377798891E-3</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19">
         <v>2.1784893392614191E-2</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F19">
         <v>-7.0100521193938697E-2</v>
       </c>
-      <c r="G19" s="2">
+      <c r="G19">
         <v>-5.8989999034612828E-2</v>
       </c>
-      <c r="H19" s="2">
+      <c r="H19">
         <v>-6.6793395665513289E-2</v>
       </c>
-      <c r="I19" s="2">
+      <c r="I19">
         <v>-1.9436566079039941E-3</v>
       </c>
-      <c r="J19" s="2">
+      <c r="J19">
         <v>-3.1913323070528149E-3</v>
       </c>
-      <c r="K19" s="2">
+      <c r="K19">
         <v>-5.2232681440545856E-3</v>
       </c>
-      <c r="L19" s="2">
+      <c r="L19">
         <v>9.9355034972768305E-2</v>
       </c>
-      <c r="M19" s="2">
+      <c r="M19">
         <v>0.10085087751752871</v>
       </c>
-      <c r="N19" s="2">
+      <c r="N19">
         <v>0.31693597717969058</v>
       </c>
-      <c r="O19" s="2">
+      <c r="O19">
         <v>0.20756372904207551</v>
       </c>
-      <c r="P19" s="2">
+      <c r="P19">
         <v>0.18124649105227689</v>
       </c>
-      <c r="Q19" s="2">
+      <c r="Q19">
         <v>0.1726629374180296</v>
       </c>
-      <c r="R19" s="2">
+      <c r="R19">
         <v>0.28557552868684261</v>
       </c>
-      <c r="S19" s="2">
-        <v>1</v>
-      </c>
-      <c r="T19" s="2">
+      <c r="S19">
+        <v>1</v>
+      </c>
+      <c r="T19">
         <v>0.24477045029284539</v>
       </c>
-      <c r="U19" s="2">
+      <c r="U19">
         <v>0.18010674364562321</v>
       </c>
-      <c r="V19" s="2">
+      <c r="V19">
         <v>0.18090775259417011</v>
       </c>
-      <c r="W19" s="2">
+      <c r="W19">
         <v>0.15763391627233669</v>
       </c>
-      <c r="X19" s="2">
+      <c r="X19">
         <v>-5.8578706582901582E-2</v>
       </c>
     </row>
@@ -1930,73 +1877,73 @@
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20">
         <v>0.210166747723388</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20">
         <v>-3.9943140867107353E-2</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20">
         <v>-3.541351946757382E-3</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20">
         <v>2.9247353045011429E-2</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20">
         <v>-7.0560837670354787E-2</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G20">
         <v>-5.5901231300968322E-2</v>
       </c>
-      <c r="H20" s="2">
+      <c r="H20">
         <v>-5.3310779586101961E-2</v>
       </c>
-      <c r="I20" s="2">
+      <c r="I20">
         <v>-6.9235203567686907E-2</v>
       </c>
-      <c r="J20" s="2">
+      <c r="J20">
         <v>9.0623626815555386E-3</v>
       </c>
-      <c r="K20" s="2">
+      <c r="K20">
         <v>5.8337741928969761E-3</v>
       </c>
-      <c r="L20" s="2">
+      <c r="L20">
         <v>0.15688713847568511</v>
       </c>
-      <c r="M20" s="2">
+      <c r="M20">
         <v>0.15071819370167511</v>
       </c>
-      <c r="N20" s="2">
+      <c r="N20">
         <v>0.1300111816244208</v>
       </c>
-      <c r="O20" s="2">
+      <c r="O20">
         <v>0.3000225291116479</v>
       </c>
-      <c r="P20" s="2">
+      <c r="P20">
         <v>0.25230486173062922</v>
       </c>
-      <c r="Q20" s="2">
+      <c r="Q20">
         <v>0.23376979332693371</v>
       </c>
-      <c r="R20" s="2">
+      <c r="R20">
         <v>0.25219113895240292</v>
       </c>
-      <c r="S20" s="2">
+      <c r="S20">
         <v>0.24477045029284539</v>
       </c>
-      <c r="T20" s="2">
-        <v>1</v>
-      </c>
-      <c r="U20" s="2">
+      <c r="T20">
+        <v>1</v>
+      </c>
+      <c r="U20">
         <v>0.2163250917008438</v>
       </c>
-      <c r="V20" s="2">
+      <c r="V20">
         <v>0.1592137203087127</v>
       </c>
-      <c r="W20" s="2">
+      <c r="W20">
         <v>0.16274003329183251</v>
       </c>
-      <c r="X20" s="2">
+      <c r="X20">
         <v>-5.6250350990331627E-2</v>
       </c>
     </row>
@@ -2004,73 +1951,73 @@
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21">
         <v>0.20324241022458289</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21">
         <v>-3.8218166111341469E-2</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21">
         <v>-1.265927889271911E-2</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21">
         <v>2.137900561558986E-2</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F21">
         <v>-6.400488888773119E-2</v>
       </c>
-      <c r="G21" s="2">
+      <c r="G21">
         <v>-4.6858411513545577E-2</v>
       </c>
-      <c r="H21" s="2">
+      <c r="H21">
         <v>-4.606653388796151E-2</v>
       </c>
-      <c r="I21" s="2">
+      <c r="I21">
         <v>-4.3461429655394422E-2</v>
       </c>
-      <c r="J21" s="2">
+      <c r="J21">
         <v>-5.829886530946838E-2</v>
       </c>
-      <c r="K21" s="2">
+      <c r="K21">
         <v>1.9017863282441622E-2</v>
       </c>
-      <c r="L21" s="2">
+      <c r="L21">
         <v>0.15830253328353999</v>
       </c>
-      <c r="M21" s="2">
+      <c r="M21">
         <v>0.14739810422001151</v>
       </c>
-      <c r="N21" s="2">
+      <c r="N21">
         <v>0.14340460499244431</v>
       </c>
-      <c r="O21" s="2">
+      <c r="O21">
         <v>0.13019140778780799</v>
       </c>
-      <c r="P21" s="2">
+      <c r="P21">
         <v>0.29311846318443119</v>
       </c>
-      <c r="Q21" s="2">
+      <c r="Q21">
         <v>0.25023682493343619</v>
       </c>
-      <c r="R21" s="2">
+      <c r="R21">
         <v>0.1995579311706798</v>
       </c>
-      <c r="S21" s="2">
+      <c r="S21">
         <v>0.18010674364562321</v>
       </c>
-      <c r="T21" s="2">
+      <c r="T21">
         <v>0.2163250917008438</v>
       </c>
-      <c r="U21" s="2">
-        <v>1</v>
-      </c>
-      <c r="V21" s="2">
+      <c r="U21">
+        <v>1</v>
+      </c>
+      <c r="V21">
         <v>0.15183043582617881</v>
       </c>
-      <c r="W21" s="2">
+      <c r="W21">
         <v>0.15783391560137269</v>
       </c>
-      <c r="X21" s="2">
+      <c r="X21">
         <v>-5.682740089288691E-2</v>
       </c>
     </row>
@@ -2078,73 +2025,73 @@
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22">
         <v>0.21720243239549611</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22">
         <v>-4.0358454928196917E-2</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22">
         <v>-1.2047569155652471E-3</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22">
         <v>2.2849973558558761E-2</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F22">
         <v>-5.8189885949777302E-2</v>
       </c>
-      <c r="G22" s="2">
+      <c r="G22">
         <v>-3.7093079770128587E-2</v>
       </c>
-      <c r="H22" s="2">
+      <c r="H22">
         <v>-3.5863070561361177E-2</v>
       </c>
-      <c r="I22" s="2">
+      <c r="I22">
         <v>-3.3589534748121493E-2</v>
       </c>
-      <c r="J22" s="2">
+      <c r="J22">
         <v>-3.333650421280087E-2</v>
       </c>
-      <c r="K22" s="2">
+      <c r="K22">
         <v>-4.6433641072996593E-2</v>
       </c>
-      <c r="L22" s="2">
+      <c r="L22">
         <v>0.16702571208291589</v>
       </c>
-      <c r="M22" s="2">
+      <c r="M22">
         <v>0.15795741162396421</v>
       </c>
-      <c r="N22" s="2">
+      <c r="N22">
         <v>0.17971235040649311</v>
       </c>
-      <c r="O22" s="2">
+      <c r="O22">
         <v>0.1604330376290044</v>
       </c>
-      <c r="P22" s="2">
+      <c r="P22">
         <v>0.14157417995960681</v>
       </c>
-      <c r="Q22" s="2">
+      <c r="Q22">
         <v>0.30772888950115462</v>
       </c>
-      <c r="R22" s="2">
+      <c r="R22">
         <v>0.1484592750153427</v>
       </c>
-      <c r="S22" s="2">
+      <c r="S22">
         <v>0.18090775259417011</v>
       </c>
-      <c r="T22" s="2">
+      <c r="T22">
         <v>0.1592137203087127</v>
       </c>
-      <c r="U22" s="2">
+      <c r="U22">
         <v>0.15183043582617881</v>
       </c>
-      <c r="V22" s="2">
-        <v>1</v>
-      </c>
-      <c r="W22" s="2">
+      <c r="V22">
+        <v>1</v>
+      </c>
+      <c r="W22">
         <v>0.15489552525961539</v>
       </c>
-      <c r="X22" s="2">
+      <c r="X22">
         <v>-5.5123515621088762E-2</v>
       </c>
     </row>
@@ -2152,73 +2099,73 @@
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23">
         <v>0.2195953686044175</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23">
         <v>-3.7199903089169373E-2</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23">
         <v>-6.640941925653474E-3</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23">
         <v>1.9478152969869801E-2</v>
       </c>
-      <c r="F23" s="2">
+      <c r="F23">
         <v>-5.8673214376070433E-2</v>
       </c>
-      <c r="G23" s="2">
+      <c r="G23">
         <v>-3.650037552721859E-2</v>
       </c>
-      <c r="H23" s="2">
+      <c r="H23">
         <v>-3.5861083718773168E-2</v>
       </c>
-      <c r="I23" s="2">
+      <c r="I23">
         <v>-2.656508796765087E-2</v>
       </c>
-      <c r="J23" s="2">
+      <c r="J23">
         <v>-2.302745098759577E-2</v>
       </c>
-      <c r="K23" s="2">
+      <c r="K23">
         <v>-2.529933846228534E-2</v>
       </c>
-      <c r="L23" s="2">
+      <c r="L23">
         <v>0.17934112200688429</v>
       </c>
-      <c r="M23" s="2">
+      <c r="M23">
         <v>0.17425616563434329</v>
       </c>
-      <c r="N23" s="2">
+      <c r="N23">
         <v>0.1823259661520534</v>
       </c>
-      <c r="O23" s="2">
+      <c r="O23">
         <v>0.17763699418674461</v>
       </c>
-      <c r="P23" s="2">
+      <c r="P23">
         <v>0.1641844503536177</v>
       </c>
-      <c r="Q23" s="2">
+      <c r="Q23">
         <v>0.1154941668516445</v>
       </c>
-      <c r="R23" s="2">
+      <c r="R23">
         <v>0.18573525544572639</v>
       </c>
-      <c r="S23" s="2">
+      <c r="S23">
         <v>0.15763391627233669</v>
       </c>
-      <c r="T23" s="2">
+      <c r="T23">
         <v>0.16274003329183251</v>
       </c>
-      <c r="U23" s="2">
+      <c r="U23">
         <v>0.15783391560137269</v>
       </c>
-      <c r="V23" s="2">
+      <c r="V23">
         <v>0.15489552525961539</v>
       </c>
-      <c r="W23" s="2">
-        <v>1</v>
-      </c>
-      <c r="X23" s="2">
+      <c r="W23">
+        <v>1</v>
+      </c>
+      <c r="X23">
         <v>-5.3183340326127961E-2</v>
       </c>
     </row>
@@ -2226,86 +2173,82 @@
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24">
         <v>-0.1535198763935072</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24">
         <v>2.8006077656250201E-2</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D24">
         <v>-2.4339215683404442E-2</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E24">
         <v>1.3889834301962891E-2</v>
       </c>
-      <c r="F24" s="2">
+      <c r="F24">
         <v>0.32479372847862242</v>
       </c>
-      <c r="G24" s="2">
+      <c r="G24">
         <v>0.26355120167216778</v>
       </c>
-      <c r="H24" s="2">
+      <c r="H24">
         <v>0.2352525137249171</v>
       </c>
-      <c r="I24" s="2">
+      <c r="I24">
         <v>0.21661363684242391</v>
       </c>
-      <c r="J24" s="2">
+      <c r="J24">
         <v>0.20414891387616449</v>
       </c>
-      <c r="K24" s="2">
+      <c r="K24">
         <v>0.18686636165354609</v>
       </c>
-      <c r="L24" s="2">
+      <c r="L24">
         <v>-1.9644197143221558E-2</v>
       </c>
-      <c r="M24" s="2">
+      <c r="M24">
         <v>-1.419321808821576E-2</v>
       </c>
-      <c r="N24" s="2">
+      <c r="N24">
         <v>-1.4075518043214731E-2</v>
       </c>
-      <c r="O24" s="2">
+      <c r="O24">
         <v>-1.0156495880289671E-2</v>
       </c>
-      <c r="P24" s="2">
+      <c r="P24">
         <v>-6.7604638410147791E-3</v>
       </c>
-      <c r="Q24" s="2">
+      <c r="Q24">
         <v>-5.3723149148155579E-3</v>
       </c>
-      <c r="R24" s="2">
+      <c r="R24">
         <v>-7.2929487777851632E-2</v>
       </c>
-      <c r="S24" s="2">
+      <c r="S24">
         <v>-5.8578706582901582E-2</v>
       </c>
-      <c r="T24" s="2">
+      <c r="T24">
         <v>-5.6250350990331627E-2</v>
       </c>
-      <c r="U24" s="2">
+      <c r="U24">
         <v>-5.682740089288691E-2</v>
       </c>
-      <c r="V24" s="2">
+      <c r="V24">
         <v>-5.5123515621088762E-2</v>
       </c>
-      <c r="W24" s="2">
+      <c r="W24">
         <v>-5.3183340326127961E-2</v>
       </c>
-      <c r="X24" s="2">
+      <c r="X24">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:X24">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="greaterThan">
+  <conditionalFormatting sqref="B2:X25">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0.75</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
-      <formula>-0.75</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>